<commit_message>
completed the inter embedded
</commit_message>
<xml_diff>
--- a/office6_performance_with_edge_result.xlsx
+++ b/office6_performance_with_edge_result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aayus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aayus\Desktop\Learning_AI_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735A5DC3-6D3E-47C6-99BF-4A3019358B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D5F17F-3D7D-488C-AEED-DE42312EEEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,10 +436,10 @@
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>